<commit_message>
Tester High Speed Sesi 1 Update!
</commit_message>
<xml_diff>
--- a/krpai2020/Tester High Speed Sesi 1/automatic calibration calculator.xlsx
+++ b/krpai2020/Tester High Speed Sesi 1/automatic calibration calculator.xlsx
@@ -1,23 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lazy_Panda\Documents\GitHub2\tirtapods-x\krpai2020\Sesi 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryano\OneDrive\Documents\GitHub\tirtapods-x\krpai2020\Sesi 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186322F3-EDB7-44E2-9DAA-AAE76443BEAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="7335" yWindow="720" windowWidth="15195" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -101,7 +108,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -506,11 +513,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,27 +613,27 @@
         <v>1400</v>
       </c>
       <c r="C4" s="1">
-        <v>1550</v>
+        <v>1430</v>
       </c>
       <c r="D4" s="1">
-        <v>1500</v>
+        <v>1600</v>
       </c>
       <c r="E4" s="1">
         <v>900</v>
       </c>
       <c r="F4" s="1">
-        <v>2000</v>
+        <v>1950</v>
       </c>
       <c r="G4" s="1">
-        <v>2000</v>
+        <v>2100</v>
       </c>
       <c r="H4" s="1">
         <f>D4-2*(D4-G4)</f>
-        <v>2500</v>
+        <v>2600</v>
       </c>
       <c r="I4" s="1">
         <f>C4</f>
-        <v>1550</v>
+        <v>1430</v>
       </c>
       <c r="J4" s="1">
         <f>E4-2*(E4-B4)</f>
@@ -638,7 +645,7 @@
       </c>
       <c r="L4" s="1">
         <f>F4-C4</f>
-        <v>450</v>
+        <v>520</v>
       </c>
       <c r="M4" s="1">
         <f>E4-B4</f>
@@ -653,27 +660,27 @@
         <v>1450</v>
       </c>
       <c r="C5" s="1">
-        <v>1600</v>
+        <v>1580</v>
       </c>
       <c r="D5" s="1">
-        <v>1400</v>
+        <v>1580</v>
       </c>
       <c r="E5" s="1">
         <v>1000</v>
       </c>
       <c r="F5" s="1">
-        <v>2070</v>
+        <v>2100</v>
       </c>
       <c r="G5" s="1">
-        <v>1850</v>
+        <v>2050</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" ref="H5:H9" si="0">D5-2*(D5-G5)</f>
-        <v>2300</v>
+        <v>2520</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" ref="I5:I9" si="1">C5</f>
-        <v>1600</v>
+        <v>1580</v>
       </c>
       <c r="J5" s="1">
         <f>B5</f>
@@ -681,11 +688,11 @@
       </c>
       <c r="K5" s="1">
         <f t="shared" ref="K5:K9" si="2">D5-G5</f>
-        <v>-450</v>
+        <v>-470</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" ref="L5:L9" si="3">F5-C5</f>
-        <v>470</v>
+        <v>520</v>
       </c>
       <c r="M5" s="1">
         <f>E5-B5</f>
@@ -697,26 +704,26 @@
         <v>3</v>
       </c>
       <c r="B6" s="1">
-        <v>1450</v>
+        <v>1350</v>
       </c>
       <c r="C6" s="1">
         <v>1400</v>
       </c>
       <c r="D6" s="1">
-        <v>1600</v>
+        <v>1680</v>
       </c>
       <c r="E6" s="1">
-        <v>950</v>
+        <v>900</v>
       </c>
       <c r="F6" s="1">
         <v>1850</v>
       </c>
       <c r="G6" s="1">
-        <v>2050</v>
+        <v>2120</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="0"/>
-        <v>2500</v>
+        <v>2560</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
@@ -724,11 +731,11 @@
       </c>
       <c r="J6" s="1">
         <f>E6</f>
-        <v>950</v>
+        <v>900</v>
       </c>
       <c r="K6" s="1">
         <f t="shared" si="2"/>
-        <v>-450</v>
+        <v>-440</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="3"/>
@@ -736,7 +743,7 @@
       </c>
       <c r="M6" s="1">
         <f>B6-E6</f>
-        <v>500</v>
+        <v>450</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -747,10 +754,10 @@
         <v>1500</v>
       </c>
       <c r="C7" s="1">
+        <v>1450</v>
+      </c>
+      <c r="D7" s="1">
         <v>1400</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1380</v>
       </c>
       <c r="E7" s="1">
         <v>2000</v>
@@ -759,15 +766,15 @@
         <v>940</v>
       </c>
       <c r="G7" s="1">
-        <v>900</v>
+        <v>850</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="0"/>
-        <v>420</v>
+        <v>300</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="1"/>
-        <v>1400</v>
+        <v>1450</v>
       </c>
       <c r="J7" s="1">
         <f>E7-2*(E7-B7)</f>
@@ -775,11 +782,11 @@
       </c>
       <c r="K7" s="1">
         <f t="shared" si="2"/>
-        <v>480</v>
+        <v>550</v>
       </c>
       <c r="L7" s="1">
         <f t="shared" si="3"/>
-        <v>-460</v>
+        <v>-510</v>
       </c>
       <c r="M7" s="1">
         <f>E7-B7</f>
@@ -794,27 +801,27 @@
         <v>1400</v>
       </c>
       <c r="C8" s="1">
-        <v>1500</v>
+        <v>1550</v>
       </c>
       <c r="D8" s="1">
-        <v>1250</v>
+        <v>1270</v>
       </c>
       <c r="E8" s="1">
-        <v>1850</v>
+        <v>1870</v>
       </c>
       <c r="F8" s="1">
         <v>1040</v>
       </c>
       <c r="G8" s="1">
-        <v>800</v>
+        <v>750</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="0"/>
-        <v>350</v>
+        <v>230</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="1"/>
-        <v>1500</v>
+        <v>1550</v>
       </c>
       <c r="J8" s="1">
         <f>B8</f>
@@ -822,15 +829,15 @@
       </c>
       <c r="K8" s="1">
         <f t="shared" si="2"/>
-        <v>450</v>
+        <v>520</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="3"/>
-        <v>-460</v>
+        <v>-510</v>
       </c>
       <c r="M8" s="1">
         <f>E8-B8</f>
-        <v>450</v>
+        <v>470</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -838,26 +845,26 @@
         <v>6</v>
       </c>
       <c r="B9" s="1">
-        <v>1300</v>
+        <v>1350</v>
       </c>
       <c r="C9" s="1">
         <v>1400</v>
       </c>
       <c r="D9" s="1">
-        <v>1400</v>
+        <v>1250</v>
       </c>
       <c r="E9" s="1">
-        <v>1800</v>
+        <v>1830</v>
       </c>
       <c r="F9" s="1">
         <v>900</v>
       </c>
       <c r="G9" s="1">
-        <v>850</v>
+        <v>750</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="1"/>
@@ -865,11 +872,11 @@
       </c>
       <c r="J9" s="1">
         <f>E9</f>
-        <v>1800</v>
+        <v>1830</v>
       </c>
       <c r="K9" s="1">
         <f t="shared" si="2"/>
-        <v>550</v>
+        <v>500</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" si="3"/>
@@ -877,7 +884,7 @@
       </c>
       <c r="M9" s="1">
         <f>B9-E9</f>
-        <v>-500</v>
+        <v>-480</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Legs on Tester Higher Speed Sesi 1!
</commit_message>
<xml_diff>
--- a/krpai2020/Tester High Speed Sesi 1/automatic calibration calculator.xlsx
+++ b/krpai2020/Tester High Speed Sesi 1/automatic calibration calculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryano\OneDrive\Documents\GitHub\tirtapods-x\krpai2020\Sesi 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DONNY\Documents\tirtapods-x\krpai2020\Sesi 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186322F3-EDB7-44E2-9DAA-AAE76443BEAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471695AA-B74D-48D0-8AD4-2A077E3144FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7335" yWindow="720" windowWidth="15195" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7875" tabRatio="442" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -517,7 +511,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,7 +610,7 @@
         <v>1430</v>
       </c>
       <c r="D4" s="1">
-        <v>1600</v>
+        <v>1580</v>
       </c>
       <c r="E4" s="1">
         <v>900</v>
@@ -625,11 +619,11 @@
         <v>1950</v>
       </c>
       <c r="G4" s="1">
-        <v>2100</v>
+        <v>2050</v>
       </c>
       <c r="H4" s="1">
         <f>D4-2*(D4-G4)</f>
-        <v>2600</v>
+        <v>2520</v>
       </c>
       <c r="I4" s="1">
         <f>C4</f>
@@ -641,7 +635,7 @@
       </c>
       <c r="K4" s="1">
         <f>D4-G4</f>
-        <v>-500</v>
+        <v>-470</v>
       </c>
       <c r="L4" s="1">
         <f>F4-C4</f>
@@ -660,27 +654,27 @@
         <v>1450</v>
       </c>
       <c r="C5" s="1">
-        <v>1580</v>
+        <v>1520</v>
       </c>
       <c r="D5" s="1">
-        <v>1580</v>
+        <v>1500</v>
       </c>
       <c r="E5" s="1">
         <v>1000</v>
       </c>
       <c r="F5" s="1">
-        <v>2100</v>
+        <v>2080</v>
       </c>
       <c r="G5" s="1">
-        <v>2050</v>
+        <v>2030</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" ref="H5:H9" si="0">D5-2*(D5-G5)</f>
-        <v>2520</v>
+        <v>2560</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" ref="I5:I9" si="1">C5</f>
-        <v>1580</v>
+        <v>1520</v>
       </c>
       <c r="J5" s="1">
         <f>B5</f>
@@ -688,11 +682,11 @@
       </c>
       <c r="K5" s="1">
         <f t="shared" ref="K5:K9" si="2">D5-G5</f>
-        <v>-470</v>
+        <v>-530</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" ref="L5:L9" si="3">F5-C5</f>
-        <v>520</v>
+        <v>560</v>
       </c>
       <c r="M5" s="1">
         <f>E5-B5</f>
@@ -707,7 +701,7 @@
         <v>1350</v>
       </c>
       <c r="C6" s="1">
-        <v>1400</v>
+        <v>1350</v>
       </c>
       <c r="D6" s="1">
         <v>1680</v>
@@ -719,15 +713,15 @@
         <v>1850</v>
       </c>
       <c r="G6" s="1">
-        <v>2120</v>
+        <v>2150</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="0"/>
-        <v>2560</v>
+        <v>2620</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>1400</v>
+        <v>1350</v>
       </c>
       <c r="J6" s="1">
         <f>E6</f>
@@ -735,11 +729,11 @@
       </c>
       <c r="K6" s="1">
         <f t="shared" si="2"/>
-        <v>-440</v>
+        <v>-470</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="3"/>
-        <v>450</v>
+        <v>500</v>
       </c>
       <c r="M6" s="1">
         <f>B6-E6</f>
@@ -754,10 +748,10 @@
         <v>1500</v>
       </c>
       <c r="C7" s="1">
-        <v>1450</v>
+        <v>1410</v>
       </c>
       <c r="D7" s="1">
-        <v>1400</v>
+        <v>1380</v>
       </c>
       <c r="E7" s="1">
         <v>2000</v>
@@ -770,11 +764,11 @@
       </c>
       <c r="H7" s="1">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="1"/>
-        <v>1450</v>
+        <v>1410</v>
       </c>
       <c r="J7" s="1">
         <f>E7-2*(E7-B7)</f>
@@ -782,11 +776,11 @@
       </c>
       <c r="K7" s="1">
         <f t="shared" si="2"/>
-        <v>550</v>
+        <v>530</v>
       </c>
       <c r="L7" s="1">
         <f t="shared" si="3"/>
-        <v>-510</v>
+        <v>-470</v>
       </c>
       <c r="M7" s="1">
         <f>E7-B7</f>
@@ -801,10 +795,10 @@
         <v>1400</v>
       </c>
       <c r="C8" s="1">
-        <v>1550</v>
+        <v>1600</v>
       </c>
       <c r="D8" s="1">
-        <v>1270</v>
+        <v>1250</v>
       </c>
       <c r="E8" s="1">
         <v>1870</v>
@@ -817,11 +811,11 @@
       </c>
       <c r="H8" s="1">
         <f t="shared" si="0"/>
-        <v>230</v>
+        <v>250</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="1"/>
-        <v>1550</v>
+        <v>1600</v>
       </c>
       <c r="J8" s="1">
         <f>B8</f>
@@ -829,11 +823,11 @@
       </c>
       <c r="K8" s="1">
         <f t="shared" si="2"/>
-        <v>520</v>
+        <v>500</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="3"/>
-        <v>-510</v>
+        <v>-560</v>
       </c>
       <c r="M8" s="1">
         <f>E8-B8</f>

</xml_diff>